<commit_message>
Clean up results sheets
</commit_message>
<xml_diff>
--- a/sheets/DEVLOG/DEVLOG_HOUR_SUMMARY-1.xlsx
+++ b/sheets/DEVLOG/DEVLOG_HOUR_SUMMARY-1.xlsx
@@ -1,12 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bakalaura_darba\sheets\DEVLOG\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE011A6-2449-46DE-961A-573575DE91B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="276" yWindow="0" windowWidth="23040" windowHeight="13644" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="DEVLOG_HOUR_SUMMARY" sheetId="1" r:id="rId4"/>
+    <sheet name="DEVLOG_HOUR_SUMMARY" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -79,16 +99,16 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
     </font>
@@ -98,7 +118,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -108,7 +128,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -122,109 +148,92 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
     <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="none"/>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFFFFFFF"/>
           <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <border/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="4" pivot="0" name="DEVLOG_HOUR_SUMMARY-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="1" type="firstRowStripe"/>
-      <tableStyleElement dxfId="1" type="secondRowStripe"/>
-      <tableStyleElement dxfId="1" type="totalRow"/>
+    <tableStyle name="DEVLOG_HOUR_SUMMARY-style" pivot="0" count="4" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="totalRow" dxfId="0"/>
+      <tableStyleElement type="firstRowStripe" dxfId="2"/>
+      <tableStyleElement type="secondRowStripe" dxfId="1"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="394308503" name="Chart1" title="Chart">
-          <a:extLst>
-            <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr preferRelativeResize="0"/>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData fLocksWithSheet="0"/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:B20" displayName="Table1" name="Table1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B20">
   <tableColumns count="2">
-    <tableColumn name="DATE" id="1"/>
-    <tableColumn name="Stundas" id="2"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="DATE"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Stundas"/>
   </tableColumns>
-  <tableStyleInfo name="DEVLOG_HOUR_SUMMARY-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="DEVLOG_HOUR_SUMMARY-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -414,23 +423,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -438,151 +450,151 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="2">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
@@ -592,9 +604,9 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>